<commit_message>
Excel de entradas y salidas mesas
</commit_message>
<xml_diff>
--- a/EntradasYSalidaMesas.xlsx
+++ b/EntradasYSalidaMesas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive\Documentos\TrabajosLocal\LogisimMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6065512F-F46F-4C71-AC99-DF2A84274139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F8DE07-FA36-42E1-B9F8-515F4AF25D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CD73D035-E036-4B7A-8835-DD23AD72DB1D}"/>
   </bookViews>
@@ -35,6 +35,104 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Ifetch</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>EX reg</t>
+  </si>
+  <si>
+    <t>Mem</t>
+  </si>
+  <si>
+    <t>Wr Register</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>Imm</t>
+  </si>
+  <si>
+    <t>Bus A</t>
+  </si>
+  <si>
+    <t>Bus B</t>
+  </si>
+  <si>
+    <t>ZERO</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>ExtOp</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>ALUOp</t>
+  </si>
+  <si>
+    <t>RegDst</t>
+  </si>
+  <si>
+    <t>MemWr</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>MemtoReg</t>
+  </si>
+  <si>
+    <t>RegWr</t>
+  </si>
+  <si>
+    <t>Dmemory</t>
+  </si>
+  <si>
+    <t>AluRespond</t>
+  </si>
+  <si>
+    <t>Mux img1</t>
+  </si>
+  <si>
+    <t>Img 1</t>
+  </si>
+  <si>
+    <t>MuxImg1</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>MemToReg</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -46,12 +144,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -81,11 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,6 +206,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>155089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>488191</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>172517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F79285D-C127-47D3-8241-60A05E69E9E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3920265"/>
+          <a:ext cx="3643767" cy="1989664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,27 +574,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE781760-52A0-44FF-8255-3E33C4C6C550}">
-  <dimension ref="B4:M4"/>
+  <dimension ref="A4:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -450,5 +825,6 @@
     <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>